<commit_message>
Added more words to the list.
</commit_message>
<xml_diff>
--- a/word_pairs/Icelandic_English_Danish_words.xlsx
+++ b/word_pairs/Icelandic_English_Danish_words.xlsx
@@ -2,44 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tumde-my.sharepoint.com/personal/selina_friesen_tum_de/Documents/Auslandssemester Dänemark/Uni/ExperimentInCognitiveScience/CognitiveExperiment/src/word_pairs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Documents\EPFL\BA5\02455_ExpCognitiveScience\CognitiveExperiment\word_pairs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B4D0E19-5B65-49C2-87F9-1B70BCD69A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A570D1-7873-4236-99D6-ACD1CA178C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{58E7559F-28CA-43ED-B0BC-D9C88FFC13C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{58E7559F-28CA-43ED-B0BC-D9C88FFC13C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
-  <si>
-    <t>#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
   <si>
     <t>Icelandic</t>
   </si>
@@ -53,9 +39,6 @@
     <t>framkvæmd</t>
   </si>
   <si>
-    <t>implementation / execution</t>
-  </si>
-  <si>
     <t>gennemførelse / udførelse</t>
   </si>
   <si>
@@ -89,18 +72,12 @@
     <t>viðhorf</t>
   </si>
   <si>
-    <t>attitude / outlook</t>
-  </si>
-  <si>
     <t>holdning</t>
   </si>
   <si>
     <t>ávinningur</t>
   </si>
   <si>
-    <t>benefit / gain</t>
-  </si>
-  <si>
     <t>udbytte / fordel</t>
   </si>
   <si>
@@ -125,9 +102,6 @@
     <t>geðshræring</t>
   </si>
   <si>
-    <t>emotion / agitation</t>
-  </si>
-  <si>
     <t>sindsbevægelse / følelse</t>
   </si>
   <si>
@@ -143,27 +117,18 @@
     <t>siðferði</t>
   </si>
   <si>
-    <t>morality / ethics</t>
-  </si>
-  <si>
     <t>moral / etik</t>
   </si>
   <si>
     <t>hugleiðing</t>
   </si>
   <si>
-    <t>meditation / contemplation</t>
-  </si>
-  <si>
     <t>meditation / overvejelse</t>
   </si>
   <si>
     <t>forsendur</t>
   </si>
   <si>
-    <t>premises / assumptions</t>
-  </si>
-  <si>
     <t>forudsætninger</t>
   </si>
   <si>
@@ -188,18 +153,12 @@
     <t>vitund</t>
   </si>
   <si>
-    <t>awareness / consciousness</t>
-  </si>
-  <si>
     <t>bevidsthed</t>
   </si>
   <si>
     <t>takmörk</t>
   </si>
   <si>
-    <t>limits / boundaries</t>
-  </si>
-  <si>
     <t>grænser</t>
   </si>
   <si>
@@ -215,9 +174,6 @@
     <t>tilfinning</t>
   </si>
   <si>
-    <t>feeling / emotion</t>
-  </si>
-  <si>
     <t>følelse</t>
   </si>
   <si>
@@ -242,18 +198,12 @@
     <t>endurreisn</t>
   </si>
   <si>
-    <t>reconstruction / revival</t>
-  </si>
-  <si>
     <t>genopbygning / genfødsel</t>
   </si>
   <si>
     <t>áhrif</t>
   </si>
   <si>
-    <t>influence / impact</t>
-  </si>
-  <si>
     <t>indflydelse / virkning</t>
   </si>
   <si>
@@ -269,9 +219,6 @@
     <t>umbreyting</t>
   </si>
   <si>
-    <t>transformation / change</t>
-  </si>
-  <si>
     <t>forvandling / omdannelse</t>
   </si>
   <si>
@@ -314,36 +261,24 @@
     <t>sambúð</t>
   </si>
   <si>
-    <t>coexistence / relationship</t>
-  </si>
-  <si>
     <t>samliv / sameksistens</t>
   </si>
   <si>
     <t>miðlun</t>
   </si>
   <si>
-    <t>mediation / communication</t>
-  </si>
-  <si>
     <t>formidling / mægling</t>
   </si>
   <si>
     <t>hlutverk</t>
   </si>
   <si>
-    <t>role / function</t>
-  </si>
-  <si>
     <t>rolle / funktion</t>
   </si>
   <si>
     <t>viðbrögð</t>
   </si>
   <si>
-    <t>reactions / response</t>
-  </si>
-  <si>
     <t>reaktioner</t>
   </si>
   <si>
@@ -359,27 +294,18 @@
     <t>arfleifð</t>
   </si>
   <si>
-    <t>heritage / legacy</t>
-  </si>
-  <si>
     <t>arv / kulturarv</t>
   </si>
   <si>
     <t>markmið</t>
   </si>
   <si>
-    <t>goal / objective</t>
-  </si>
-  <si>
     <t>mål / målsætning</t>
   </si>
   <si>
     <t>áhrifaríkur</t>
   </si>
   <si>
-    <t>influential / effective</t>
-  </si>
-  <si>
     <t>indflydelsesrig / effektiv</t>
   </si>
   <si>
@@ -395,19 +321,184 @@
     <t>hvatning</t>
   </si>
   <si>
-    <t>encouragement / motivation</t>
-  </si>
-  <si>
     <t>opmuntring / motivation</t>
   </si>
   <si>
     <t>samkennd</t>
   </si>
   <si>
-    <t>empathy / compassion</t>
-  </si>
-  <si>
     <t>empati / medfølelse</t>
+  </si>
+  <si>
+    <t>camel</t>
+  </si>
+  <si>
+    <t>úlfaldi</t>
+  </si>
+  <si>
+    <t>moon</t>
+  </si>
+  <si>
+    <t>tungl</t>
+  </si>
+  <si>
+    <t>flame</t>
+  </si>
+  <si>
+    <t>logi</t>
+  </si>
+  <si>
+    <t>smile</t>
+  </si>
+  <si>
+    <t>bros</t>
+  </si>
+  <si>
+    <t>shark</t>
+  </si>
+  <si>
+    <t>hákarl</t>
+  </si>
+  <si>
+    <t>cigar</t>
+  </si>
+  <si>
+    <t>vindlingur</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>sími</t>
+  </si>
+  <si>
+    <t>sheep</t>
+  </si>
+  <si>
+    <t>sauðfé</t>
+  </si>
+  <si>
+    <t>pistol</t>
+  </si>
+  <si>
+    <t>skammbyssa</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>ljósmynd</t>
+  </si>
+  <si>
+    <t>daisy</t>
+  </si>
+  <si>
+    <t>margísla</t>
+  </si>
+  <si>
+    <t>purse</t>
+  </si>
+  <si>
+    <t>veski</t>
+  </si>
+  <si>
+    <t>kamel</t>
+  </si>
+  <si>
+    <t>måne</t>
+  </si>
+  <si>
+    <t>flamme</t>
+  </si>
+  <si>
+    <t>smil</t>
+  </si>
+  <si>
+    <t>haj</t>
+  </si>
+  <si>
+    <t>cigaret</t>
+  </si>
+  <si>
+    <t>telefon</t>
+  </si>
+  <si>
+    <t>får</t>
+  </si>
+  <si>
+    <t>fotografi</t>
+  </si>
+  <si>
+    <t>flere gidsler</t>
+  </si>
+  <si>
+    <t>pung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementation </t>
+  </si>
+  <si>
+    <t>attitude</t>
+  </si>
+  <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>emotion</t>
+  </si>
+  <si>
+    <t>ethics</t>
+  </si>
+  <si>
+    <t>meditation</t>
+  </si>
+  <si>
+    <t>assumptions</t>
+  </si>
+  <si>
+    <t>awareness</t>
+  </si>
+  <si>
+    <t>limits</t>
+  </si>
+  <si>
+    <t>feeling</t>
+  </si>
+  <si>
+    <t>reconstruction</t>
+  </si>
+  <si>
+    <t>influence</t>
+  </si>
+  <si>
+    <t>coexistence</t>
+  </si>
+  <si>
+    <t>transformation</t>
+  </si>
+  <si>
+    <t>mediation</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>reactions</t>
+  </si>
+  <si>
+    <t>heritage</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>influential</t>
+  </si>
+  <si>
+    <t>motivation</t>
+  </si>
+  <si>
+    <t>empathy</t>
   </si>
 </sst>
 </file>
@@ -461,7 +552,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -793,19 +884,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA451DF-899A-4660-AA88-EF4BDB7BBC09}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,568 +907,577 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
       <c r="B2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="2" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="2" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="2" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="2" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="2" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>28</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="2" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="B31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>29</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>34</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>35</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>36</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>37</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>39</v>
-      </c>
-      <c r="B32" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>40</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="B40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>41</v>
-      </c>
-      <c r="B34" s="2" t="s">
+      <c r="B41" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>42</v>
-      </c>
-      <c r="B35" s="2" t="s">
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>44</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="C44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>45</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="C45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C46" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <v>47</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>48</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>49</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="C50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>50</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
         <v>121</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
         <v>123</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1385,6 +1486,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010084B226A5A1FAD74BBFCCAF6F06C8958F" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="99a855a5ba9ab20f45b3cafb9116f5af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="90d25a49-44c1-4e51-912b-582f89f599b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4cd0dfb4c73e2227168b250139cc678" ns3:_="">
     <xsd:import namespace="90d25a49-44c1-4e51-912b-582f89f599b4"/>
@@ -1598,15 +1708,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1616,6 +1717,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB40A05F-B4F6-40F2-B572-F3BB1D7A99E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7067B3D-843E-417B-98F0-DEA5721C3954}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1629,14 +1738,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB40A05F-B4F6-40F2-B572-F3BB1D7A99E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Word list has been reduced to exactly 50 word pairs. Results are corrected for 25 word instead of 50
</commit_message>
<xml_diff>
--- a/word_pairs/Icelandic_English_Danish_words.xlsx
+++ b/word_pairs/Icelandic_English_Danish_words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Documents\EPFL\BA5\02455_ExpCognitiveScience\CognitiveExperiment\word_pairs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venello/Repositories/Python/PyCharm/PycharmProjects/CognitiveExperiment/word_pairs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A570D1-7873-4236-99D6-ACD1CA178C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9698F9F3-4C4C-4945-8898-85EB15F09A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{58E7559F-28CA-43ED-B0BC-D9C88FFC13C3}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="25880" windowHeight="17260" xr2:uid="{58E7559F-28CA-43ED-B0BC-D9C88FFC13C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="152">
   <si>
     <t>Icelandic</t>
   </si>
@@ -309,15 +309,6 @@
     <t>indflydelsesrig / effektiv</t>
   </si>
   <si>
-    <t>réttlæti</t>
-  </si>
-  <si>
-    <t>justice</t>
-  </si>
-  <si>
-    <t>retfærdighed</t>
-  </si>
-  <si>
     <t>hvatning</t>
   </si>
   <si>
@@ -390,12 +381,6 @@
     <t>ljósmynd</t>
   </si>
   <si>
-    <t>daisy</t>
-  </si>
-  <si>
-    <t>margísla</t>
-  </si>
-  <si>
     <t>purse</t>
   </si>
   <si>
@@ -427,9 +412,6 @@
   </si>
   <si>
     <t>fotografi</t>
-  </si>
-  <si>
-    <t>flere gidsler</t>
   </si>
   <si>
     <t>pung</t>
@@ -884,20 +866,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA451DF-899A-4660-AA88-EF4BDB7BBC09}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,18 +890,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -930,7 +912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -941,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -952,29 +934,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -985,7 +967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -996,18 +978,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1018,40 +1000,40 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -1062,7 +1044,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
@@ -1073,29 +1055,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1106,18 +1088,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1128,7 +1110,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -1139,29 +1121,29 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -1172,18 +1154,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
@@ -1194,7 +1176,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>68</v>
       </c>
@@ -1205,7 +1187,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>71</v>
       </c>
@@ -1216,7 +1198,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
@@ -1227,51 +1209,51 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>85</v>
       </c>
@@ -1282,202 +1264,180 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="B40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
         <v>102</v>
       </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>116</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>124</v>
-      </c>
-      <c r="B53" t="s">
-        <v>123</v>
-      </c>
-      <c r="C53" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1486,15 +1446,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010084B226A5A1FAD74BBFCCAF6F06C8958F" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="99a855a5ba9ab20f45b3cafb9116f5af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="90d25a49-44c1-4e51-912b-582f89f599b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4cd0dfb4c73e2227168b250139cc678" ns3:_="">
     <xsd:import namespace="90d25a49-44c1-4e51-912b-582f89f599b4"/>
@@ -1708,6 +1659,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1717,14 +1677,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB40A05F-B4F6-40F2-B572-F3BB1D7A99E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7067B3D-843E-417B-98F0-DEA5721C3954}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1738,6 +1690,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB40A05F-B4F6-40F2-B572-F3BB1D7A99E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>